<commit_message>
Update GitHub Actions workflow for Python tests
</commit_message>
<xml_diff>
--- a/book_data.xlsx
+++ b/book_data.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -661,25 +661,75 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>システム設計の面接試験</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>アレックス　シユウ</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="0" t="n">
         <v>2800</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>Kindle</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>未定</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>ハンズオンで学ぶAWSコスト最適化入門</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>緒方遼太郎</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>Kindle</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>未定</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>テスト書籍</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>テスト著者</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>単行本</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>未定</t>
         </is>

</xml_diff>